<commit_message>
Last Changes for CRUISE
</commit_message>
<xml_diff>
--- a/cruise_grade.xlsx
+++ b/cruise_grade.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AD49CE-D281-4782-8DE6-752A85B24349}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5F0EF5-CB2A-44B6-B18E-C186BE17CD07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9252" yWindow="1500" windowWidth="13788" windowHeight="8424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="107">
   <si>
     <t>Dirt6</t>
   </si>
@@ -440,6 +440,10 @@
   </si>
   <si>
     <t>2.0.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>89.30？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1000,12 +1004,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M159"/>
+  <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J164" sqref="J164"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4400,6 +4404,14 @@
       <c r="K159" s="29">
         <f>SUM(E159:J159)</f>
         <v>694.32</v>
+      </c>
+    </row>
+    <row r="161" spans="6:7">
+      <c r="F161" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G161" s="2">
+        <v>127.39</v>
       </c>
     </row>
   </sheetData>
@@ -8429,5 +8441,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>